<commit_message>
Added compiled data and analysis
</commit_message>
<xml_diff>
--- a/Chaos Tests/Phase Plot.xlsx
+++ b/Chaos Tests/Phase Plot.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\American Work\2018 FALL\Phys Capstone\Chaos Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\American Work\2018 FALL\Phys Capstone\ChaosPendulum\Chaos Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992AEA2A-64E0-445E-9587-E60769E37EE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D59AB1D-A1D0-4A86-AF31-4BC8CFC57BC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5802" xr2:uid="{B6B1692E-65CE-40FB-8AAC-9B9060B63F63}"/>
   </bookViews>
@@ -117,7 +117,75 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Finding</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> the Greatest Damping</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40949300087489071"/>
+          <c:y val="1.2746972594008922E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -125,7 +193,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.14167825896762903"/>
-          <c:y val="5.0925925925925923E-2"/>
+          <c:y val="9.3415904273916051E-2"/>
           <c:w val="0.81232174103237098"/>
           <c:h val="0.74350320793234181"/>
         </c:manualLayout>
@@ -266,73 +334,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.75901328273244784</c:v>
+                  <c:v>1.3174999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75614366729678639</c:v>
+                  <c:v>1.3225</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75187969924812026</c:v>
+                  <c:v>1.33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76804915514592942</c:v>
+                  <c:v>1.302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.76687116564417179</c:v>
+                  <c:v>1.3039999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75414781297134237</c:v>
+                  <c:v>1.3260000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.77922077922077926</c:v>
+                  <c:v>1.2833333333333334</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.77519379844961234</c:v>
+                  <c:v>1.29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77419354838709675</c:v>
+                  <c:v>1.2916666666666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.76923076923076927</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.76824583866837393</c:v>
+                  <c:v>1.3016666666666665</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.76824583866837393</c:v>
+                  <c:v>1.3016666666666665</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.76726342710997442</c:v>
+                  <c:v>1.3033333333333335</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.76628352490421459</c:v>
+                  <c:v>1.3049999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.76238881829733163</c:v>
+                  <c:v>1.3116666666666668</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.75187969924812026</c:v>
+                  <c:v>1.33</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.76004343105320293</c:v>
+                  <c:v>1.3157142857142858</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.77041602465331271</c:v>
+                  <c:v>1.298</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.76745970836531086</c:v>
+                  <c:v>1.3029999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.75815011372251706</c:v>
+                  <c:v>1.319</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.75131480090157776</c:v>
+                  <c:v>1.331</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.74682598954443613</c:v>
+                  <c:v>1.339</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.73900726690479124</c:v>
+                  <c:v>1.3531666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -402,7 +470,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.73900726690479124</c:v>
+                  <c:v>1.3531666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1276,16 +1344,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>97155</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>97155</xdr:rowOff>
+      <xdr:rowOff>169545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1613,7 +1681,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1653,12 +1721,12 @@
         <v>0.82</v>
       </c>
       <c r="D2">
-        <f>A2/B2</f>
-        <v>0.75901328273244784</v>
+        <f>B2/A2</f>
+        <v>1.3174999999999999</v>
       </c>
       <c r="E2">
-        <f>2*PI()/D2</f>
-        <v>8.2780966422091051</v>
+        <f t="shared" ref="E2:E24" si="0">2*PI()/D2</f>
+        <v>4.7690211060186618</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1672,12 +1740,12 @@
         <v>1.66</v>
       </c>
       <c r="D3">
-        <f>A3/B3</f>
-        <v>0.75614366729678639</v>
+        <f t="shared" ref="D3:D24" si="1">B3/A3</f>
+        <v>1.3225</v>
       </c>
       <c r="E3">
-        <f>2*PI()/D3</f>
-        <v>8.3095125687450029</v>
+        <f t="shared" si="0"/>
+        <v>4.7509907804760578</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1691,12 +1759,12 @@
         <v>1.04</v>
       </c>
       <c r="D4">
-        <f>A4/B4</f>
-        <v>0.75187969924812026</v>
+        <f t="shared" si="1"/>
+        <v>1.33</v>
       </c>
       <c r="E4">
-        <f>2*PI()/D4</f>
-        <v>8.3566364585488504</v>
+        <f t="shared" si="0"/>
+        <v>4.7241994790823956</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1710,12 +1778,12 @@
         <v>1.28</v>
       </c>
       <c r="D5">
-        <f>A5/B5</f>
-        <v>0.76804915514592942</v>
+        <f t="shared" si="1"/>
+        <v>1.302</v>
       </c>
       <c r="E5">
-        <f>2*PI()/D5</f>
-        <v>8.1807072699478205</v>
+        <f t="shared" si="0"/>
+        <v>4.825795166804598</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1729,12 +1797,12 @@
         <v>2.72</v>
       </c>
       <c r="D6">
-        <f>A6/B6</f>
-        <v>0.76687116564417179</v>
+        <f t="shared" si="1"/>
+        <v>1.3039999999999998</v>
       </c>
       <c r="E6">
-        <f>2*PI()/D6</f>
-        <v>8.1932736405621807</v>
+        <f t="shared" si="0"/>
+        <v>4.8183936404751435</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1748,12 +1816,12 @@
         <v>9.0399999999999991</v>
       </c>
       <c r="D7">
-        <f>A7/B7</f>
-        <v>0.75414781297134237</v>
+        <f t="shared" si="1"/>
+        <v>1.3260000000000001</v>
       </c>
       <c r="E7">
-        <f>2*PI()/D7</f>
-        <v>8.3315037173201318</v>
+        <f t="shared" si="0"/>
+        <v>4.7384504579031566</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1767,12 +1835,12 @@
         <v>3.35</v>
       </c>
       <c r="D8">
-        <f>A8/B8</f>
-        <v>0.77922077922077926</v>
+        <f t="shared" si="1"/>
+        <v>1.2833333333333334</v>
       </c>
       <c r="E8">
-        <f>2*PI()/D8</f>
-        <v>8.0634211442138017</v>
+        <f t="shared" si="0"/>
+        <v>4.8959885510490277</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1786,12 +1854,12 @@
         <v>3.01</v>
       </c>
       <c r="D9">
-        <f>A9/B9</f>
-        <v>0.77519379844961234</v>
+        <f t="shared" si="1"/>
+        <v>1.29</v>
       </c>
       <c r="E9">
-        <f>2*PI()/D9</f>
-        <v>8.1053090462616666</v>
+        <f t="shared" si="0"/>
+        <v>4.8706862846353376</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1805,12 +1873,12 @@
         <v>2.15</v>
       </c>
       <c r="D10">
-        <f>A10/B10</f>
-        <v>0.77419354838709675</v>
+        <f t="shared" si="1"/>
+        <v>1.2916666666666667</v>
       </c>
       <c r="E10">
-        <f>2*PI()/D10</f>
-        <v>8.1157810217736319</v>
+        <f t="shared" si="0"/>
+        <v>4.8644015281390338</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1824,12 +1892,12 @@
         <v>2.54</v>
       </c>
       <c r="D11">
-        <f>A11/B11</f>
-        <v>0.76923076923076927</v>
+        <f t="shared" si="1"/>
+        <v>1.3</v>
       </c>
       <c r="E11">
-        <f>2*PI()/D11</f>
-        <v>8.1681408993334621</v>
+        <f t="shared" si="0"/>
+        <v>4.8332194670612196</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1843,12 +1911,12 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="D12">
-        <f>A12/B12</f>
-        <v>0.76824583866837393</v>
+        <f t="shared" si="1"/>
+        <v>1.3016666666666665</v>
       </c>
       <c r="E12">
-        <f>2*PI()/D12</f>
-        <v>8.1786128748454274</v>
+        <f t="shared" si="0"/>
+        <v>4.8270309658229857</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1862,12 +1930,12 @@
         <v>4.3899999999999997</v>
       </c>
       <c r="D13">
-        <f>A13/B13</f>
-        <v>0.76824583866837393</v>
+        <f t="shared" si="1"/>
+        <v>1.3016666666666665</v>
       </c>
       <c r="E13">
-        <f>2*PI()/D13</f>
-        <v>8.1786128748454274</v>
+        <f t="shared" si="0"/>
+        <v>4.8270309658229857</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1881,12 +1949,12 @@
         <v>3.37</v>
       </c>
       <c r="D14">
-        <f>A14/B14</f>
-        <v>0.76726342710997442</v>
+        <f t="shared" si="1"/>
+        <v>1.3033333333333335</v>
       </c>
       <c r="E14">
-        <f>2*PI()/D14</f>
-        <v>8.1890848503573945</v>
+        <f t="shared" si="0"/>
+        <v>4.8208582919536465</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1900,12 +1968,12 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="D15">
-        <f>A15/B15</f>
-        <v>0.76628352490421459</v>
+        <f t="shared" si="1"/>
+        <v>1.3049999999999999</v>
       </c>
       <c r="E15">
-        <f>2*PI()/D15</f>
-        <v>8.1995568258693599</v>
+        <f t="shared" si="0"/>
+        <v>4.8147013848119435</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1919,12 +1987,12 @@
         <v>6.01</v>
       </c>
       <c r="D16">
-        <f>A16/B16</f>
-        <v>0.76238881829733163</v>
+        <f t="shared" si="1"/>
+        <v>1.3116666666666668</v>
       </c>
       <c r="E16">
-        <f>2*PI()/D16</f>
-        <v>8.2414447279172247</v>
+        <f t="shared" si="0"/>
+        <v>4.7902302214838013</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1938,12 +2006,12 @@
         <v>7.92</v>
       </c>
       <c r="D17">
-        <f>A17/B17</f>
-        <v>0.75187969924812026</v>
+        <f t="shared" si="1"/>
+        <v>1.33</v>
       </c>
       <c r="E17">
-        <f>2*PI()/D17</f>
-        <v>8.3566364585488504</v>
+        <f t="shared" si="0"/>
+        <v>4.7241994790823956</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1957,12 +2025,12 @@
         <v>6.96</v>
       </c>
       <c r="D18">
-        <f>A18/B18</f>
-        <v>0.76004343105320293</v>
+        <f t="shared" si="1"/>
+        <v>1.3157142857142858</v>
       </c>
       <c r="E18">
-        <f>2*PI()/D18</f>
-        <v>8.2668766684462849</v>
+        <f t="shared" si="0"/>
+        <v>4.7754937188118456</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1976,12 +2044,12 @@
         <v>6.56</v>
       </c>
       <c r="D19">
-        <f>A19/B19</f>
-        <v>0.77041602465331271</v>
+        <f t="shared" si="1"/>
+        <v>1.298</v>
       </c>
       <c r="E19">
-        <f>2*PI()/D19</f>
-        <v>8.1555745287191037</v>
+        <f t="shared" si="0"/>
+        <v>4.8406666465174002</v>
       </c>
       <c r="G19">
         <v>10</v>
@@ -1993,12 +2061,12 @@
         <v>15</v>
       </c>
       <c r="J19">
-        <f>G19/H19</f>
-        <v>0.7412898443291327</v>
+        <f>H19/G19</f>
+        <v>1.349</v>
       </c>
       <c r="K19">
-        <f>2*PI()/J19</f>
-        <v>8.4760169793852622</v>
+        <f t="shared" ref="K19:K24" si="2">2*PI()/J19</f>
+        <v>4.6576614582502494</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2012,12 +2080,12 @@
         <v>5.14</v>
       </c>
       <c r="D20">
-        <f>A20/B20</f>
-        <v>0.76745970836531086</v>
+        <f t="shared" si="1"/>
+        <v>1.3029999999999999</v>
       </c>
       <c r="E20">
-        <f>2*PI()/D20</f>
-        <v>8.1869904552549997</v>
+        <f t="shared" si="0"/>
+        <v>4.8220915634532515</v>
       </c>
       <c r="G20">
         <v>10</v>
@@ -2029,12 +2097,12 @@
         <v>15</v>
       </c>
       <c r="J20">
-        <f>G20/H20</f>
-        <v>0.73964497041420119</v>
+        <f t="shared" ref="J20:J24" si="3">H20/G20</f>
+        <v>1.3519999999999999</v>
       </c>
       <c r="K20">
-        <f>2*PI()/J20</f>
-        <v>8.4948665353067998</v>
+        <f t="shared" si="2"/>
+        <v>4.647326410635789</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2048,12 +2116,12 @@
         <v>8.93</v>
       </c>
       <c r="D21">
-        <f>A21/B21</f>
-        <v>0.75815011372251706</v>
+        <f t="shared" si="1"/>
+        <v>1.319</v>
       </c>
       <c r="E21">
-        <f>2*PI()/D21</f>
-        <v>8.2875214201698739</v>
+        <f t="shared" si="0"/>
+        <v>4.7635976551778514</v>
       </c>
       <c r="G21">
         <v>10</v>
@@ -2065,12 +2133,12 @@
         <v>15</v>
       </c>
       <c r="J21">
-        <f>G21/H21</f>
-        <v>0.74404761904761907</v>
+        <f t="shared" si="3"/>
+        <v>1.3439999999999999</v>
       </c>
       <c r="K21">
-        <f>2*PI()/J21</f>
-        <v>8.4446010528493645</v>
+        <f t="shared" si="2"/>
+        <v>4.6749890678419543</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2084,12 +2152,12 @@
         <v>11.21</v>
       </c>
       <c r="D22">
-        <f>A22/B22</f>
-        <v>0.75131480090157776</v>
+        <f t="shared" si="1"/>
+        <v>1.331</v>
       </c>
       <c r="E22">
-        <f>2*PI()/D22</f>
-        <v>8.3629196438560296</v>
+        <f t="shared" si="0"/>
+        <v>4.72065011809135</v>
       </c>
       <c r="G22">
         <v>10</v>
@@ -2101,12 +2169,12 @@
         <v>15</v>
       </c>
       <c r="J22">
-        <f>G22/H22</f>
-        <v>0.73529411764705888</v>
+        <f t="shared" si="3"/>
+        <v>1.3599999999999999</v>
       </c>
       <c r="K22">
-        <f>2*PI()/J22</f>
-        <v>8.5451320177642369</v>
+        <f t="shared" si="2"/>
+        <v>4.6199891964555784</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2120,12 +2188,12 @@
         <v>10.7</v>
       </c>
       <c r="D23">
-        <f>A23/B23</f>
-        <v>0.74682598954443613</v>
+        <f t="shared" si="1"/>
+        <v>1.339</v>
       </c>
       <c r="E23">
-        <f>2*PI()/D23</f>
-        <v>8.4131851263134667</v>
+        <f t="shared" si="0"/>
+        <v>4.6924460845254563</v>
       </c>
       <c r="G23">
         <v>10</v>
@@ -2137,12 +2205,12 @@
         <v>15</v>
       </c>
       <c r="J23">
-        <f>G23/H23</f>
-        <v>0.73691967575534267</v>
+        <f t="shared" si="3"/>
+        <v>1.357</v>
       </c>
       <c r="K23">
-        <f>2*PI()/J23</f>
-        <v>8.5262824618426993</v>
+        <f t="shared" si="2"/>
+        <v>4.6302028792775136</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2157,12 +2225,12 @@
         <v>0.5</v>
       </c>
       <c r="D24">
-        <f>A24/B24</f>
-        <v>0.73900726690479124</v>
+        <f>B24/A24</f>
+        <v>1.3531666666666666</v>
       </c>
       <c r="E24">
-        <f>2*PI()/D24</f>
-        <v>8.5021969181651773</v>
+        <f t="shared" si="0"/>
+        <v>4.6433196013151274</v>
       </c>
       <c r="G24">
         <v>10</v>
@@ -2174,12 +2242,12 @@
         <v>15</v>
       </c>
       <c r="J24">
-        <f>G24/H24</f>
-        <v>0.73691967575534267</v>
+        <f t="shared" si="3"/>
+        <v>1.357</v>
       </c>
       <c r="K24">
-        <f>2*PI()/J24</f>
-        <v>8.5262824618426993</v>
+        <f t="shared" si="2"/>
+        <v>4.6302028792775136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>